<commit_message>
fix: fix media infor
</commit_message>
<xml_diff>
--- a/backend/utils/Childhood_Content.xlsx
+++ b/backend/utils/Childhood_Content.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="7575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="7575" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tom&amp;Jerry" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="846">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="845">
   <si>
     <t>Link</t>
   </si>
@@ -2544,9 +2544,6 @@
   </si>
   <si>
     <t>https://drive.google.com/file/d/1M8iJq9aCYWcC7MERaGMlnpKVYH5m-R3q/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>END</t>
   </si>
   <si>
     <t>https://drive.google.com/file/d/1eIIJaO1x6GYjHzjk4hmokEVEOIvF4Mhr/view?usp=sharing</t>
@@ -3025,7 +3022,7 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A383" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -3038,10 +3035,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -9551,7 +9548,7 @@
   </sheetPr>
   <dimension ref="A1:Z13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -9564,10 +9561,10 @@
   <sheetData>
     <row r="1" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>0</v>
@@ -9754,8 +9751,8 @@
   </sheetPr>
   <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9766,7 +9763,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="B1" s="23" t="s">
         <v>0</v>
@@ -10133,11 +10130,11 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="9">
+        <v>46</v>
+      </c>
+      <c r="B47" s="11" t="s">
         <v>841</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>842</v>
       </c>
     </row>
   </sheetData>

</xml_diff>